<commit_message>
add auto evaluation function
</commit_message>
<xml_diff>
--- a/experiment/Experiment Record.xlsx
+++ b/experiment/Experiment Record.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420" activeTab="2"/>
+    <workbookView windowWidth="22368" windowHeight="9420" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="MRR" sheetId="2" r:id="rId2"/>
     <sheet name="score2" sheetId="3" r:id="rId3"/>
+    <sheet name="auto evalulation" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
   <si>
     <t>vote/603,604</t>
   </si>
@@ -708,13 +709,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1073,8 +1074,8 @@
   <sheetPr/>
   <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1124,10 +1125,10 @@
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="2" t="s">
@@ -1205,12 +1206,12 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="3">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B3" s="2">
         <v>602</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>603</v>
       </c>
       <c r="D3" s="2">
@@ -1225,7 +1226,7 @@
       <c r="G3" s="2">
         <v>403</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>402</v>
       </c>
       <c r="I3" s="3">
@@ -1237,19 +1238,19 @@
       <c r="K3" s="2">
         <v>602</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>602</v>
       </c>
       <c r="M3" s="3">
         <v>503</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>503</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="3">
         <v>503</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="3">
         <v>401</v>
       </c>
       <c r="Q3" s="2">
@@ -1267,55 +1268,55 @@
       <c r="U3" s="3">
         <v>401</v>
       </c>
-      <c r="V3" s="4">
+      <c r="V3" s="3">
         <v>401</v>
       </c>
-      <c r="W3" s="4">
+      <c r="W3" s="3">
         <v>401</v>
       </c>
-      <c r="X3" s="4">
+      <c r="X3" s="3">
         <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="3">
-        <v>603</v>
-      </c>
-      <c r="B4" s="4">
+        <v>604</v>
+      </c>
+      <c r="B4" s="3">
         <v>603</v>
       </c>
       <c r="C4" s="2">
         <v>602</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>603</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>402</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>402</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>402</v>
       </c>
       <c r="H4" s="2">
         <v>403</v>
       </c>
       <c r="I4" s="2">
-        <v>602</v>
-      </c>
-      <c r="J4" s="4">
+        <v>604</v>
+      </c>
+      <c r="J4" s="3">
         <v>603</v>
       </c>
       <c r="K4" s="2">
         <v>604</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>603</v>
       </c>
       <c r="M4" s="2">
-        <v>402</v>
+        <v>502</v>
       </c>
       <c r="N4" s="2">
         <v>502</v>
@@ -1335,19 +1336,19 @@
       <c r="S4" s="2">
         <v>306</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="3">
         <v>302</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="3">
         <v>402</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="3">
         <v>402</v>
       </c>
-      <c r="W4" s="4">
+      <c r="W4" s="3">
         <v>402</v>
       </c>
-      <c r="X4" s="4">
+      <c r="X4" s="3">
         <v>402</v>
       </c>
     </row>
@@ -1355,13 +1356,13 @@
       <c r="A5" s="2">
         <v>602</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>604</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>604</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>604</v>
       </c>
       <c r="E5" s="2"/>
@@ -1369,19 +1370,19 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="J5" s="2">
         <v>604</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>603</v>
       </c>
       <c r="L5" s="2">
         <v>604</v>
       </c>
       <c r="M5" s="2">
-        <v>502</v>
+        <v>402</v>
       </c>
       <c r="N5" s="2">
         <v>402</v>
@@ -1389,7 +1390,7 @@
       <c r="O5" s="2">
         <v>403</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="5">
         <v>501</v>
       </c>
       <c r="Q5" s="2">
@@ -1401,7 +1402,7 @@
       <c r="S5" s="2">
         <v>501</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5" s="3">
         <v>303</v>
       </c>
       <c r="U5" s="8">
@@ -1430,32 +1431,32 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="2">
-        <v>501</v>
-      </c>
-      <c r="N6" s="4">
+      <c r="M6" s="6">
+        <v>401</v>
+      </c>
+      <c r="N6" s="3">
         <v>401</v>
       </c>
       <c r="O6" s="2">
         <v>501</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="3">
         <v>503</v>
       </c>
       <c r="Q6" s="2">
         <v>305</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="3">
         <v>303</v>
       </c>
       <c r="S6" s="2">
         <v>201</v>
       </c>
-      <c r="T6" s="4">
+      <c r="T6" s="3">
         <v>304</v>
       </c>
       <c r="U6" s="8">
-        <v>504</v>
+        <v>403</v>
       </c>
       <c r="V6" s="2">
         <v>501</v>
@@ -1480,13 +1481,13 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="3">
-        <v>401</v>
+      <c r="M7" s="5">
+        <v>501</v>
       </c>
       <c r="N7" s="2">
         <v>403</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>401</v>
       </c>
       <c r="P7" s="2">
@@ -1505,7 +1506,7 @@
         <v>305</v>
       </c>
       <c r="U7" s="2">
-        <v>403</v>
+        <v>504</v>
       </c>
       <c r="V7" s="2">
         <v>502</v>
@@ -1545,10 +1546,10 @@
       <c r="Q8" s="3">
         <v>303</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R8" s="3">
         <v>304</v>
       </c>
-      <c r="S8" s="4">
+      <c r="S8" s="3">
         <v>303</v>
       </c>
       <c r="T8" s="2">
@@ -1587,10 +1588,10 @@
       <c r="Q9" s="2">
         <v>306</v>
       </c>
-      <c r="R9" s="4">
+      <c r="R9" s="3">
         <v>302</v>
       </c>
-      <c r="S9" s="4">
+      <c r="S9" s="3">
         <v>302</v>
       </c>
       <c r="T9" s="2">
@@ -1624,7 +1625,7 @@
       <c r="R10" s="2">
         <v>504</v>
       </c>
-      <c r="S10" s="4">
+      <c r="S10" s="3">
         <v>304</v>
       </c>
       <c r="T10" s="2">
@@ -1818,8 +1819,8 @@
   <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1873,4 +1874,65 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="11.3333333333333" customWidth="1"/>
+    <col min="2" max="2" width="9.66666666666667"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.451886</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.4963</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.6119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.5297</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update inverse page freqency algorithm
</commit_message>
<xml_diff>
--- a/experiment/Experiment Record.xlsx
+++ b/experiment/Experiment Record.xlsx
@@ -696,7 +696,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -713,9 +713,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1405,7 +1402,7 @@
       <c r="T5" s="3">
         <v>303</v>
       </c>
-      <c r="U5" s="8">
+      <c r="U5" s="7">
         <v>501</v>
       </c>
       <c r="V5" s="2">
@@ -1431,7 +1428,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="6">
+      <c r="M6" s="3">
         <v>401</v>
       </c>
       <c r="N6" s="3">
@@ -1455,7 +1452,7 @@
       <c r="T6" s="3">
         <v>304</v>
       </c>
-      <c r="U6" s="8">
+      <c r="U6" s="7">
         <v>403</v>
       </c>
       <c r="V6" s="2">
@@ -1716,7 +1713,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="7"/>
+      <c r="L13" s="6"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1882,7 +1879,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1928,7 +1925,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="1">
-        <v>0.5297</v>
+        <v>0.5866</v>
       </c>
     </row>
   </sheetData>

</xml_diff>